<commit_message>
Update for final export
</commit_message>
<xml_diff>
--- a/natural-conversion/ESA_CCI_Natural_Conversion_Coding_v2.xlsx
+++ b/natural-conversion/ESA_CCI_Natural_Conversion_Coding_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\LandDegradation\sbtn-land-hub\natural-conversion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E25C1F3-81A8-40B1-99A8-283552195939}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44B6DBFD-9555-411C-8523-F4EC469A89A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{823A0E91-CB45-46FA-AF87-3C9F5C01C171}"/>
   </bookViews>
@@ -618,7 +618,34 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="0"/>
@@ -952,7 +979,10 @@
   <dimension ref="A1:AO41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+      <pane xSplit="4" ySplit="4" topLeftCell="S25" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomRight" activeCell="AJ35" sqref="AJ35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.5" x14ac:dyDescent="0.35"/>
@@ -1963,7 +1993,7 @@
         <v>0</v>
       </c>
       <c r="AJ9" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AK9" s="3">
         <v>1</v>
@@ -2005,7 +2035,7 @@
         <v>1</v>
       </c>
       <c r="I10" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J10" s="3">
         <v>0</v>
@@ -2086,7 +2116,7 @@
         <v>0</v>
       </c>
       <c r="AJ10" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AK10" s="3">
         <v>1</v>
@@ -3346,22 +3376,22 @@
         <v>-1</v>
       </c>
       <c r="E21" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F21" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G21" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H21" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I21" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J21" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K21" s="3">
         <v>0</v>
@@ -3439,7 +3469,7 @@
         <v>0</v>
       </c>
       <c r="AJ21" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK21" s="3">
         <v>0</v>
@@ -3469,22 +3499,22 @@
         <v>-1</v>
       </c>
       <c r="E22" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F22" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G22" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H22" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I22" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J22" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K22" s="3">
         <v>0</v>
@@ -3562,7 +3592,7 @@
         <v>0</v>
       </c>
       <c r="AJ22" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK22" s="3">
         <v>0</v>
@@ -3685,7 +3715,7 @@
         <v>0</v>
       </c>
       <c r="AJ23" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AK23" s="3">
         <v>1</v>
@@ -3808,7 +3838,7 @@
         <v>0</v>
       </c>
       <c r="AJ24" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AK24" s="3">
         <v>1</v>
@@ -3931,7 +3961,7 @@
         <v>0</v>
       </c>
       <c r="AJ25" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AK25" s="3">
         <v>1</v>
@@ -4054,7 +4084,7 @@
         <v>0</v>
       </c>
       <c r="AJ26" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AK26" s="3">
         <v>1</v>
@@ -4177,7 +4207,7 @@
         <v>0</v>
       </c>
       <c r="AJ27" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AK27" s="3">
         <v>1</v>
@@ -4300,7 +4330,7 @@
         <v>0</v>
       </c>
       <c r="AJ28" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AK28" s="3">
         <v>1</v>
@@ -4423,7 +4453,7 @@
         <v>0</v>
       </c>
       <c r="AJ29" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AK29" s="3">
         <v>1</v>
@@ -4546,7 +4576,7 @@
         <v>0</v>
       </c>
       <c r="AJ30" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AK30" s="3">
         <v>1</v>
@@ -4669,7 +4699,7 @@
         <v>0</v>
       </c>
       <c r="AJ31" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AK31" s="3">
         <v>1</v>
@@ -4792,7 +4822,7 @@
         <v>0</v>
       </c>
       <c r="AJ32" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AK32" s="3">
         <v>1</v>
@@ -4915,7 +4945,7 @@
         <v>0</v>
       </c>
       <c r="AJ33" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AK33" s="3">
         <v>1</v>
@@ -5038,7 +5068,7 @@
         <v>0</v>
       </c>
       <c r="AJ34" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AK34" s="3">
         <v>1</v>
@@ -5161,7 +5191,7 @@
         <v>0</v>
       </c>
       <c r="AJ35" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AK35" s="3">
         <v>1</v>
@@ -5923,11 +5953,14 @@
     <mergeCell ref="D1:AO1"/>
   </mergeCells>
   <conditionalFormatting sqref="D4:AO41">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>-1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update for final calculations
</commit_message>
<xml_diff>
--- a/natural-conversion/ESA_CCI_Natural_Conversion_Coding_v2.xlsx
+++ b/natural-conversion/ESA_CCI_Natural_Conversion_Coding_v2.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\LandDegradation\sbtn-land-hub\natural-conversion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44B6DBFD-9555-411C-8523-F4EC469A89A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4EC7163-44CC-465B-9751-13A7DFC9A76A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{823A0E91-CB45-46FA-AF87-3C9F5C01C171}"/>
   </bookViews>
   <sheets>
-    <sheet name="Recoding" sheetId="1" r:id="rId1"/>
+    <sheet name="Legend" sheetId="2" r:id="rId1"/>
+    <sheet name="Recoding" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="44">
   <si>
     <t>Permanent snow and ice</t>
   </si>
@@ -155,12 +156,24 @@
   <si>
     <t>Final State</t>
   </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>Class</t>
+  </si>
+  <si>
+    <t>Recode</t>
+  </si>
+  <si>
+    <t>Note that 0 indicates no data,  1 indicates "natural", 2 indicates forest, 3 indicates "cropland ", 4 indicates "urban", 5 indicates "other"</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -184,6 +197,14 @@
     </font>
     <font>
       <sz val="48"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -396,7 +417,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
@@ -608,6 +629,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
@@ -618,7 +650,153 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="20">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="0"/>
@@ -643,26 +821,6 @@
       <fill>
         <patternFill>
           <bgColor theme="7" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -975,67 +1133,541 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C7D6D4D-9A35-4167-B48A-56370BEC8D81}">
+  <dimension ref="A1:C40"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="37" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" style="75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C1" s="72" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="71" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="71" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="73" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>0</v>
+      </c>
+      <c r="B3" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>10</v>
+      </c>
+      <c r="B4" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="74">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>11</v>
+      </c>
+      <c r="B5" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="74">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>12</v>
+      </c>
+      <c r="B6" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="74">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>20</v>
+      </c>
+      <c r="B7" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="74">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>30</v>
+      </c>
+      <c r="B8" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="74">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>40</v>
+      </c>
+      <c r="B9" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>50</v>
+      </c>
+      <c r="B10" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="74">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>60</v>
+      </c>
+      <c r="B11" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="74">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>61</v>
+      </c>
+      <c r="B12" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="74">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>62</v>
+      </c>
+      <c r="B13" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="74">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>70</v>
+      </c>
+      <c r="B14" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="74">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>71</v>
+      </c>
+      <c r="B15" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="74">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>72</v>
+      </c>
+      <c r="B16" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="74">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>80</v>
+      </c>
+      <c r="B17" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="74">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>81</v>
+      </c>
+      <c r="B18" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="74">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>82</v>
+      </c>
+      <c r="B19" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="74">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>90</v>
+      </c>
+      <c r="B20" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="74">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>100</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="74">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>110</v>
+      </c>
+      <c r="B22" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" s="74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>120</v>
+      </c>
+      <c r="B23" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" s="74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>121</v>
+      </c>
+      <c r="B24" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24" s="74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>122</v>
+      </c>
+      <c r="B25" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>130</v>
+      </c>
+      <c r="B26" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" s="74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>140</v>
+      </c>
+      <c r="B27" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" s="74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>150</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C28" s="74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <v>151</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" s="74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
+        <v>152</v>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C30" s="74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <v>153</v>
+      </c>
+      <c r="B31" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" s="74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>160</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32" s="74">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
+        <v>170</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C33" s="74">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
+        <v>180</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C34" s="74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
+        <v>190</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35" s="74">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="2">
+        <v>200</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C36" s="74">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="2">
+        <v>201</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C37" s="74">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="2">
+        <v>202</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C38" s="74">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="2">
+        <v>210</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C39" s="74">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="2">
+        <v>220</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C40" s="74">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="C1:C1048576">
+    <cfRule type="cellIs" dxfId="11" priority="3" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="4" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="5" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="6" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
+      <formula>5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BCB0EB6-C292-4B5C-9670-CF75DFEBA3B5}">
   <dimension ref="A1:AO41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="S25" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="4" ySplit="4" topLeftCell="E17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AJ35" sqref="AJ35"/>
+      <selection pane="bottomRight" activeCell="E38" sqref="A1:AO41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.54296875" customWidth="1"/>
-    <col min="2" max="2" width="9.1796875" style="2"/>
-    <col min="3" max="3" width="25.81640625" style="1" customWidth="1"/>
-    <col min="4" max="41" width="15.7265625" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="2"/>
+    <col min="3" max="3" width="25.85546875" style="1" customWidth="1"/>
+    <col min="4" max="41" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" ht="61.5" x14ac:dyDescent="0.35">
-      <c r="D1" s="72" t="s">
+    <row r="1" spans="1:41" ht="61.5" x14ac:dyDescent="0.25">
+      <c r="D1" s="77" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
-      <c r="G1" s="72"/>
-      <c r="H1" s="72"/>
-      <c r="I1" s="72"/>
-      <c r="J1" s="72"/>
-      <c r="K1" s="72"/>
-      <c r="L1" s="72"/>
-      <c r="M1" s="72"/>
-      <c r="N1" s="72"/>
-      <c r="O1" s="72"/>
-      <c r="P1" s="72"/>
-      <c r="Q1" s="72"/>
-      <c r="R1" s="72"/>
-      <c r="S1" s="72"/>
-      <c r="T1" s="72"/>
-      <c r="U1" s="72"/>
-      <c r="V1" s="72"/>
-      <c r="W1" s="72"/>
-      <c r="X1" s="72"/>
-      <c r="Y1" s="72"/>
-      <c r="Z1" s="72"/>
-      <c r="AA1" s="72"/>
-      <c r="AB1" s="72"/>
-      <c r="AC1" s="72"/>
-      <c r="AD1" s="72"/>
-      <c r="AE1" s="72"/>
-      <c r="AF1" s="72"/>
-      <c r="AG1" s="72"/>
-      <c r="AH1" s="72"/>
-      <c r="AI1" s="72"/>
-      <c r="AJ1" s="72"/>
-      <c r="AK1" s="72"/>
-      <c r="AL1" s="72"/>
-      <c r="AM1" s="72"/>
-      <c r="AN1" s="72"/>
-      <c r="AO1" s="72"/>
-    </row>
-    <row r="2" spans="1:41" s="69" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
+      <c r="I1" s="77"/>
+      <c r="J1" s="77"/>
+      <c r="K1" s="77"/>
+      <c r="L1" s="77"/>
+      <c r="M1" s="77"/>
+      <c r="N1" s="77"/>
+      <c r="O1" s="77"/>
+      <c r="P1" s="77"/>
+      <c r="Q1" s="77"/>
+      <c r="R1" s="77"/>
+      <c r="S1" s="77"/>
+      <c r="T1" s="77"/>
+      <c r="U1" s="77"/>
+      <c r="V1" s="77"/>
+      <c r="W1" s="77"/>
+      <c r="X1" s="77"/>
+      <c r="Y1" s="77"/>
+      <c r="Z1" s="77"/>
+      <c r="AA1" s="77"/>
+      <c r="AB1" s="77"/>
+      <c r="AC1" s="77"/>
+      <c r="AD1" s="77"/>
+      <c r="AE1" s="77"/>
+      <c r="AF1" s="77"/>
+      <c r="AG1" s="77"/>
+      <c r="AH1" s="77"/>
+      <c r="AI1" s="77"/>
+      <c r="AJ1" s="77"/>
+      <c r="AK1" s="77"/>
+      <c r="AL1" s="77"/>
+      <c r="AM1" s="77"/>
+      <c r="AN1" s="77"/>
+      <c r="AO1" s="77"/>
+    </row>
+    <row r="2" spans="1:41" s="69" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B2" s="2"/>
       <c r="C2" s="70"/>
       <c r="D2" s="69">
@@ -1153,7 +1785,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="3" spans="1:41" s="35" customFormat="1" ht="91.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:41" s="35" customFormat="1" ht="91.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="68"/>
       <c r="C3" s="67"/>
       <c r="D3" s="66" t="s">
@@ -1271,8 +1903,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:41" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="71" t="s">
+    <row r="4" spans="1:41" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="76" t="s">
         <v>38</v>
       </c>
       <c r="B4" s="2">
@@ -1396,8 +2028,8 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="5" spans="1:41" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="71"/>
+    <row r="5" spans="1:41" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="76"/>
       <c r="B5" s="2">
         <v>10</v>
       </c>
@@ -1519,8 +2151,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:41" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="71"/>
+    <row r="6" spans="1:41" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="76"/>
       <c r="B6" s="2">
         <v>11</v>
       </c>
@@ -1642,8 +2274,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:41" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="71"/>
+    <row r="7" spans="1:41" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="76"/>
       <c r="B7" s="2">
         <v>12</v>
       </c>
@@ -1765,8 +2397,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:41" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="71"/>
+    <row r="8" spans="1:41" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="76"/>
       <c r="B8" s="2">
         <v>20</v>
       </c>
@@ -1888,8 +2520,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:41" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="71"/>
+    <row r="9" spans="1:41" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="76"/>
       <c r="B9" s="2">
         <v>30</v>
       </c>
@@ -2011,8 +2643,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:41" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="71"/>
+    <row r="10" spans="1:41" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="76"/>
       <c r="B10" s="2">
         <v>40</v>
       </c>
@@ -2134,8 +2766,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:41" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="71"/>
+    <row r="11" spans="1:41" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="76"/>
       <c r="B11" s="2">
         <v>50</v>
       </c>
@@ -2257,8 +2889,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:41" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="71"/>
+    <row r="12" spans="1:41" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="76"/>
       <c r="B12" s="2">
         <v>60</v>
       </c>
@@ -2380,8 +3012,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:41" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="71"/>
+    <row r="13" spans="1:41" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="76"/>
       <c r="B13" s="2">
         <v>61</v>
       </c>
@@ -2503,8 +3135,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:41" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="71"/>
+    <row r="14" spans="1:41" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="76"/>
       <c r="B14" s="2">
         <v>62</v>
       </c>
@@ -2626,8 +3258,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:41" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="71"/>
+    <row r="15" spans="1:41" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="76"/>
       <c r="B15" s="2">
         <v>70</v>
       </c>
@@ -2749,8 +3381,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:41" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="71"/>
+    <row r="16" spans="1:41" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="76"/>
       <c r="B16" s="2">
         <v>71</v>
       </c>
@@ -2872,8 +3504,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:41" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="71"/>
+    <row r="17" spans="1:41" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="76"/>
       <c r="B17" s="2">
         <v>72</v>
       </c>
@@ -2995,8 +3627,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:41" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="71"/>
+    <row r="18" spans="1:41" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="76"/>
       <c r="B18" s="2">
         <v>80</v>
       </c>
@@ -3118,8 +3750,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:41" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="71"/>
+    <row r="19" spans="1:41" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="76"/>
       <c r="B19" s="2">
         <v>81</v>
       </c>
@@ -3241,8 +3873,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:41" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="71"/>
+    <row r="20" spans="1:41" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="76"/>
       <c r="B20" s="2">
         <v>82</v>
       </c>
@@ -3364,8 +3996,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:41" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="71"/>
+    <row r="21" spans="1:41" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="76"/>
       <c r="B21" s="2">
         <v>90</v>
       </c>
@@ -3487,8 +4119,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:41" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="71"/>
+    <row r="22" spans="1:41" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="76"/>
       <c r="B22" s="2">
         <v>100</v>
       </c>
@@ -3610,8 +4242,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:41" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="71"/>
+    <row r="23" spans="1:41" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="76"/>
       <c r="B23" s="2">
         <v>110</v>
       </c>
@@ -3733,8 +4365,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:41" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="71"/>
+    <row r="24" spans="1:41" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="76"/>
       <c r="B24" s="2">
         <v>120</v>
       </c>
@@ -3856,8 +4488,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:41" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="71"/>
+    <row r="25" spans="1:41" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="76"/>
       <c r="B25" s="2">
         <v>121</v>
       </c>
@@ -3979,8 +4611,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:41" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="71"/>
+    <row r="26" spans="1:41" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="76"/>
       <c r="B26" s="2">
         <v>122</v>
       </c>
@@ -4102,8 +4734,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:41" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="71"/>
+    <row r="27" spans="1:41" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="76"/>
       <c r="B27" s="2">
         <v>130</v>
       </c>
@@ -4225,8 +4857,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:41" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="71"/>
+    <row r="28" spans="1:41" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="76"/>
       <c r="B28" s="2">
         <v>140</v>
       </c>
@@ -4348,8 +4980,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:41" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="71"/>
+    <row r="29" spans="1:41" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="76"/>
       <c r="B29" s="2">
         <v>150</v>
       </c>
@@ -4471,8 +5103,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:41" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="71"/>
+    <row r="30" spans="1:41" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="76"/>
       <c r="B30" s="2">
         <v>151</v>
       </c>
@@ -4594,8 +5226,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:41" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="71"/>
+    <row r="31" spans="1:41" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="76"/>
       <c r="B31" s="2">
         <v>152</v>
       </c>
@@ -4717,8 +5349,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:41" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="71"/>
+    <row r="32" spans="1:41" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="76"/>
       <c r="B32" s="2">
         <v>153</v>
       </c>
@@ -4840,8 +5472,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:41" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="71"/>
+    <row r="33" spans="1:41" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="76"/>
       <c r="B33" s="2">
         <v>160</v>
       </c>
@@ -4963,8 +5595,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:41" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="71"/>
+    <row r="34" spans="1:41" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="76"/>
       <c r="B34" s="2">
         <v>170</v>
       </c>
@@ -5086,8 +5718,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:41" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="71"/>
+    <row r="35" spans="1:41" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="76"/>
       <c r="B35" s="2">
         <v>180</v>
       </c>
@@ -5209,8 +5841,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:41" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="71"/>
+    <row r="36" spans="1:41" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="76"/>
       <c r="B36" s="2">
         <v>190</v>
       </c>
@@ -5332,8 +5964,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:41" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="71"/>
+    <row r="37" spans="1:41" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="76"/>
       <c r="B37" s="2">
         <v>200</v>
       </c>
@@ -5455,8 +6087,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:41" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="71"/>
+    <row r="38" spans="1:41" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="76"/>
       <c r="B38" s="2">
         <v>201</v>
       </c>
@@ -5578,8 +6210,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:41" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="71"/>
+    <row r="39" spans="1:41" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="76"/>
       <c r="B39" s="2">
         <v>202</v>
       </c>
@@ -5701,8 +6333,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:41" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="71"/>
+    <row r="40" spans="1:41" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="76"/>
       <c r="B40" s="2">
         <v>210</v>
       </c>
@@ -5824,8 +6456,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:41" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="71"/>
+    <row r="41" spans="1:41" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="76"/>
       <c r="B41" s="2">
         <v>220</v>
       </c>
@@ -5953,14 +6585,14 @@
     <mergeCell ref="D1:AO1"/>
   </mergeCells>
   <conditionalFormatting sqref="D4:AO41">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="1" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="2" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="3" operator="equal">
       <formula>-1</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
-      <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add function to recode initial cover layer
</commit_message>
<xml_diff>
--- a/natural-conversion/ESA_CCI_Natural_Conversion_Coding_v2.xlsx
+++ b/natural-conversion/ESA_CCI_Natural_Conversion_Coding_v2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\LandDegradation\sbtn-land-hub\natural-conversion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4EC7163-44CC-465B-9751-13A7DFC9A76A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D535145-1899-45B3-8503-28599761BC43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{823A0E91-CB45-46FA-AF87-3C9F5C01C171}"/>
+    <workbookView xWindow="20" yWindow="460" windowWidth="25580" windowHeight="13940" xr2:uid="{823A0E91-CB45-46FA-AF87-3C9F5C01C171}"/>
   </bookViews>
   <sheets>
     <sheet name="Legend" sheetId="2" r:id="rId1"/>
@@ -650,21 +650,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="20">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="9">
     <dxf>
       <font>
         <color theme="0"/>
@@ -677,28 +663,18 @@
     </dxf>
     <dxf>
       <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color theme="0"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
+          <bgColor rgb="FFC00000"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
+          <bgColor theme="7" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
     </dxf>
@@ -750,77 +726,6 @@
       <fill>
         <patternFill>
           <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1136,8 +1041,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C7D6D4D-9A35-4167-B48A-56370BEC8D81}">
   <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1582,22 +1487,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="11" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>5</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1611,10 +1516,10 @@
   <dimension ref="A1:AO41"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="E17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="4" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="E38" sqref="A1:AO41"/>
+      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
@@ -6585,13 +6490,13 @@
     <mergeCell ref="D1:AO1"/>
   </mergeCells>
   <conditionalFormatting sqref="D4:AO41">
-    <cfRule type="cellIs" dxfId="19" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
       <formula>-1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>